<commit_message>
New Expression based strategy
Pending Cemi Case validation
</commit_message>
<xml_diff>
--- a/CEMI_refuerzos.xlsx
+++ b/CEMI_refuerzos.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpern\Documents\GitHub\PyFlow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56367\Documents\GitHub\PyFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CBCEDB-3F5F-47BB-84A0-0F20EEF77017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277660A6-F5C7-475F-BEE6-FB4C4BC654CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MBOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MBOM!$A$1:$D$99</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="124">
   <si>
     <t>Time</t>
   </si>
@@ -134,230 +134,299 @@
     <t>_126</t>
   </si>
   <si>
-    <t>_127</t>
-  </si>
-  <si>
     <t>_128</t>
   </si>
   <si>
     <t>_129</t>
   </si>
   <si>
-    <t>_130</t>
-  </si>
-  <si>
-    <t>_131</t>
-  </si>
-  <si>
-    <t>_132</t>
-  </si>
-  <si>
-    <t>_133</t>
-  </si>
-  <si>
-    <t>_134</t>
-  </si>
-  <si>
-    <t>_135</t>
-  </si>
-  <si>
-    <t>_136</t>
-  </si>
-  <si>
     <t>_137</t>
   </si>
   <si>
-    <t>_138</t>
-  </si>
-  <si>
-    <t>_139</t>
-  </si>
-  <si>
-    <t>_140</t>
-  </si>
-  <si>
-    <t>_141</t>
-  </si>
-  <si>
-    <t>_142</t>
-  </si>
-  <si>
-    <t>_143</t>
-  </si>
-  <si>
-    <t>_144</t>
-  </si>
-  <si>
-    <t>_145</t>
-  </si>
-  <si>
-    <t>_146</t>
-  </si>
-  <si>
-    <t>_147</t>
-  </si>
-  <si>
-    <t>_148</t>
-  </si>
-  <si>
-    <t>_149</t>
-  </si>
-  <si>
-    <t>_150</t>
-  </si>
-  <si>
-    <t>_151</t>
-  </si>
-  <si>
-    <t>_152</t>
-  </si>
-  <si>
-    <t>_153</t>
-  </si>
-  <si>
-    <t>_154</t>
-  </si>
-  <si>
-    <t>_155</t>
-  </si>
-  <si>
-    <t>_156</t>
-  </si>
-  <si>
-    <t>_157</t>
-  </si>
-  <si>
-    <t>_158</t>
-  </si>
-  <si>
-    <t>_159</t>
-  </si>
-  <si>
-    <t>_160</t>
-  </si>
-  <si>
-    <t>_161</t>
-  </si>
-  <si>
-    <t>_162</t>
-  </si>
-  <si>
-    <t>_163</t>
-  </si>
-  <si>
-    <t>_164</t>
-  </si>
-  <si>
-    <t>_165</t>
-  </si>
-  <si>
-    <t>_166</t>
-  </si>
-  <si>
-    <t>_167</t>
-  </si>
-  <si>
-    <t>_168</t>
-  </si>
-  <si>
-    <t>_169</t>
-  </si>
-  <si>
-    <t>_170</t>
-  </si>
-  <si>
-    <t>_171</t>
-  </si>
-  <si>
-    <t>_172</t>
-  </si>
-  <si>
-    <t>_173</t>
-  </si>
-  <si>
-    <t>_174</t>
-  </si>
-  <si>
-    <t>_175</t>
-  </si>
-  <si>
-    <t>_176</t>
-  </si>
-  <si>
-    <t>_177</t>
-  </si>
-  <si>
-    <t>_178</t>
-  </si>
-  <si>
-    <t>_179</t>
-  </si>
-  <si>
-    <t>_180</t>
-  </si>
-  <si>
-    <t>_181</t>
-  </si>
-  <si>
-    <t>_182</t>
-  </si>
-  <si>
-    <t>_183</t>
-  </si>
-  <si>
-    <t>_184</t>
-  </si>
-  <si>
-    <t>_185</t>
-  </si>
-  <si>
-    <t>_186</t>
-  </si>
-  <si>
-    <t>_187</t>
-  </si>
-  <si>
-    <t>_188</t>
-  </si>
-  <si>
-    <t>_189</t>
-  </si>
-  <si>
-    <t>_190</t>
-  </si>
-  <si>
-    <t>_191</t>
-  </si>
-  <si>
-    <t>_192</t>
-  </si>
-  <si>
-    <t>_193</t>
-  </si>
-  <si>
-    <t>_194</t>
-  </si>
-  <si>
-    <t>_195</t>
-  </si>
-  <si>
-    <t>_196</t>
-  </si>
-  <si>
-    <t>_199</t>
-  </si>
-  <si>
-    <t>Refuerzo</t>
+    <t>Refuerzo1</t>
+  </si>
+  <si>
+    <t>Refuerzo2</t>
+  </si>
+  <si>
+    <t>Refuerzo3</t>
+  </si>
+  <si>
+    <t>Refuerzo4</t>
+  </si>
+  <si>
+    <t>Refuerzo5</t>
+  </si>
+  <si>
+    <t>Refuerzo6</t>
+  </si>
+  <si>
+    <t>Refuerzo7</t>
+  </si>
+  <si>
+    <t>Refuerzo8</t>
+  </si>
+  <si>
+    <t>Refuerzo9</t>
+  </si>
+  <si>
+    <t>Refuerzo10</t>
+  </si>
+  <si>
+    <t>Refuerzo11</t>
+  </si>
+  <si>
+    <t>Refuerzo12</t>
+  </si>
+  <si>
+    <t>Refuerzo13</t>
+  </si>
+  <si>
+    <t>Refuerzo14</t>
+  </si>
+  <si>
+    <t>Refuerzo15</t>
+  </si>
+  <si>
+    <t>Refuerzo16</t>
+  </si>
+  <si>
+    <t>Refuerzo17</t>
+  </si>
+  <si>
+    <t>Refuerzo18</t>
+  </si>
+  <si>
+    <t>Refuerzo19</t>
+  </si>
+  <si>
+    <t>Refuerzo20</t>
+  </si>
+  <si>
+    <t>Refuerzo21</t>
+  </si>
+  <si>
+    <t>Refuerzo22</t>
+  </si>
+  <si>
+    <t>Refuerzo23</t>
+  </si>
+  <si>
+    <t>Refuerzo24</t>
+  </si>
+  <si>
+    <t>Refuerzo25</t>
+  </si>
+  <si>
+    <t>Refuerzo26</t>
+  </si>
+  <si>
+    <t>Refuerzo27</t>
+  </si>
+  <si>
+    <t>Refuerzo28</t>
+  </si>
+  <si>
+    <t>Refuerzo29</t>
+  </si>
+  <si>
+    <t>Refuerzo30</t>
+  </si>
+  <si>
+    <t>Refuerzo31</t>
+  </si>
+  <si>
+    <t>Refuerzo32</t>
+  </si>
+  <si>
+    <t>Refuerzo33</t>
+  </si>
+  <si>
+    <t>Refuerzo34</t>
+  </si>
+  <si>
+    <t>Refuerzo35</t>
+  </si>
+  <si>
+    <t>Refuerzo36</t>
+  </si>
+  <si>
+    <t>Refuerzo37</t>
+  </si>
+  <si>
+    <t>Refuerzo38</t>
+  </si>
+  <si>
+    <t>Refuerzo39</t>
+  </si>
+  <si>
+    <t>Refuerzo40</t>
+  </si>
+  <si>
+    <t>Refuerzo41</t>
+  </si>
+  <si>
+    <t>Refuerzo42</t>
+  </si>
+  <si>
+    <t>Refuerzo43</t>
+  </si>
+  <si>
+    <t>Refuerzo44</t>
+  </si>
+  <si>
+    <t>Refuerzo45</t>
+  </si>
+  <si>
+    <t>Refuerzo46</t>
+  </si>
+  <si>
+    <t>Refuerzo47</t>
+  </si>
+  <si>
+    <t>Refuerzo48</t>
+  </si>
+  <si>
+    <t>Refuerzo49</t>
+  </si>
+  <si>
+    <t>Refuerzo50</t>
+  </si>
+  <si>
+    <t>Refuerzo51</t>
+  </si>
+  <si>
+    <t>Refuerzo52</t>
+  </si>
+  <si>
+    <t>Refuerzo53</t>
+  </si>
+  <si>
+    <t>Refuerzo54</t>
+  </si>
+  <si>
+    <t>Refuerzo55</t>
+  </si>
+  <si>
+    <t>Refuerzo56</t>
+  </si>
+  <si>
+    <t>Refuerzo57</t>
+  </si>
+  <si>
+    <t>Refuerzo58</t>
+  </si>
+  <si>
+    <t>Refuerzo59</t>
+  </si>
+  <si>
+    <t>Refuerzo60</t>
+  </si>
+  <si>
+    <t>Refuerzo61</t>
+  </si>
+  <si>
+    <t>Refuerzo62</t>
+  </si>
+  <si>
+    <t>Refuerzo63</t>
+  </si>
+  <si>
+    <t>Refuerzo64</t>
+  </si>
+  <si>
+    <t>Refuerzo65</t>
+  </si>
+  <si>
+    <t>Refuerzo66</t>
+  </si>
+  <si>
+    <t>Refuerzo67</t>
+  </si>
+  <si>
+    <t>Refuerzo68</t>
+  </si>
+  <si>
+    <t>Refuerzo69</t>
+  </si>
+  <si>
+    <t>Refuerzo70</t>
+  </si>
+  <si>
+    <t>Refuerzo71</t>
+  </si>
+  <si>
+    <t>Refuerzo72</t>
+  </si>
+  <si>
+    <t>Refuerzo73</t>
+  </si>
+  <si>
+    <t>Refuerzo74</t>
+  </si>
+  <si>
+    <t>Refuerzo75</t>
+  </si>
+  <si>
+    <t>Refuerzo76</t>
+  </si>
+  <si>
+    <t>Refuerzo77</t>
+  </si>
+  <si>
+    <t>Refuerzo78</t>
+  </si>
+  <si>
+    <t>Refuerzo79</t>
+  </si>
+  <si>
+    <t>Refuerzo80</t>
+  </si>
+  <si>
+    <t>Refuerzo81</t>
+  </si>
+  <si>
+    <t>Refuerzo82</t>
+  </si>
+  <si>
+    <t>Refuerzo83</t>
+  </si>
+  <si>
+    <t>Refuerzo84</t>
+  </si>
+  <si>
+    <t>Refuerzo85</t>
+  </si>
+  <si>
+    <t>Refuerzo86</t>
+  </si>
+  <si>
+    <t>Refuerzo87</t>
+  </si>
+  <si>
+    <t>Refuerzo88</t>
+  </si>
+  <si>
+    <t>Refuerzo89</t>
+  </si>
+  <si>
+    <t>Refuerzo90</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -665,13 +734,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J91" sqref="J91"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -692,13 +764,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -706,13 +778,13 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -720,13 +792,13 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -734,13 +806,13 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -748,13 +820,13 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -762,13 +834,13 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>39</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -776,13 +848,13 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -790,13 +862,13 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -804,13 +876,13 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -818,13 +890,13 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -832,13 +904,13 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -846,13 +918,13 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -860,13 +932,13 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -874,13 +946,13 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -888,13 +960,13 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -902,13 +974,13 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -916,13 +988,13 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>50</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -930,13 +1002,13 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -944,13 +1016,13 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -958,13 +1030,13 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -972,13 +1044,13 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -986,13 +1058,13 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>55</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1000,13 +1072,13 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1014,13 +1086,13 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1028,13 +1100,13 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1042,13 +1114,13 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1056,13 +1128,13 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>60</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1070,13 +1142,13 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1084,13 +1156,13 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1098,13 +1170,13 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1112,13 +1184,13 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1126,13 +1198,13 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1140,13 +1212,13 @@
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1154,13 +1226,13 @@
         <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1168,13 +1240,13 @@
         <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1182,13 +1254,13 @@
         <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1196,13 +1268,13 @@
         <v>0</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1210,13 +1282,13 @@
         <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1224,13 +1296,13 @@
         <v>0</v>
       </c>
       <c r="B40" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1238,13 +1310,13 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1252,13 +1324,13 @@
         <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1266,13 +1338,13 @@
         <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="C43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1280,13 +1352,13 @@
         <v>0</v>
       </c>
       <c r="B44" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1294,13 +1366,13 @@
         <v>0</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="C45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1308,13 +1380,13 @@
         <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1322,13 +1394,13 @@
         <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1336,13 +1408,13 @@
         <v>0</v>
       </c>
       <c r="B48" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1350,13 +1422,13 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="C49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1364,13 +1436,13 @@
         <v>0</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1378,13 +1450,13 @@
         <v>0</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1392,13 +1464,13 @@
         <v>0</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1406,13 +1478,13 @@
         <v>0</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1420,13 +1492,13 @@
         <v>0</v>
       </c>
       <c r="B54" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1434,13 +1506,13 @@
         <v>0</v>
       </c>
       <c r="B55" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1448,13 +1520,13 @@
         <v>0</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1462,13 +1534,13 @@
         <v>0</v>
       </c>
       <c r="B57" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1476,13 +1548,13 @@
         <v>0</v>
       </c>
       <c r="B58" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1490,13 +1562,13 @@
         <v>0</v>
       </c>
       <c r="B59" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1504,13 +1576,13 @@
         <v>0</v>
       </c>
       <c r="B60" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1518,13 +1590,13 @@
         <v>0</v>
       </c>
       <c r="B61" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1532,13 +1604,13 @@
         <v>0</v>
       </c>
       <c r="B62" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1546,13 +1618,13 @@
         <v>0</v>
       </c>
       <c r="B63" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1560,13 +1632,13 @@
         <v>0</v>
       </c>
       <c r="B64" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1574,13 +1646,13 @@
         <v>0</v>
       </c>
       <c r="B65" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1588,13 +1660,13 @@
         <v>0</v>
       </c>
       <c r="B66" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1602,13 +1674,13 @@
         <v>0</v>
       </c>
       <c r="B67" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1616,13 +1688,13 @@
         <v>0</v>
       </c>
       <c r="B68" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
       <c r="D68" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1630,13 +1702,13 @@
         <v>0</v>
       </c>
       <c r="B69" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1650,7 +1722,7 @@
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1658,13 +1730,13 @@
         <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1672,13 +1744,13 @@
         <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
       <c r="D72" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1686,13 +1758,13 @@
         <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -1700,13 +1772,13 @@
         <v>0</v>
       </c>
       <c r="B74" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
       <c r="D74" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1714,13 +1786,13 @@
         <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -1728,13 +1800,13 @@
         <v>0</v>
       </c>
       <c r="B76" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -1742,13 +1814,13 @@
         <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -1756,13 +1828,13 @@
         <v>0</v>
       </c>
       <c r="B78" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -1770,13 +1842,13 @@
         <v>0</v>
       </c>
       <c r="B79" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -1784,13 +1856,13 @@
         <v>0</v>
       </c>
       <c r="B80" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -1798,13 +1870,13 @@
         <v>0</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -1812,13 +1884,13 @@
         <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -1826,13 +1898,13 @@
         <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C83">
         <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -1840,13 +1912,13 @@
         <v>0</v>
       </c>
       <c r="B84" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="C84">
         <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>86</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -1854,13 +1926,13 @@
         <v>0</v>
       </c>
       <c r="B85" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="C85">
         <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>87</v>
+        <v>33</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -1868,13 +1940,13 @@
         <v>0</v>
       </c>
       <c r="B86" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="C86">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -1882,13 +1954,13 @@
         <v>0</v>
       </c>
       <c r="B87" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="C87">
         <v>1</v>
       </c>
       <c r="D87" t="s">
-        <v>89</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -1896,13 +1968,13 @@
         <v>0</v>
       </c>
       <c r="B88" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="C88">
         <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -1910,13 +1982,13 @@
         <v>0</v>
       </c>
       <c r="B89" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="C89">
         <v>1</v>
       </c>
       <c r="D89" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -1924,13 +1996,13 @@
         <v>0</v>
       </c>
       <c r="B90" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="C90">
         <v>1</v>
       </c>
       <c r="D90" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -1938,133 +2010,17 @@
         <v>0</v>
       </c>
       <c r="B91" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="C91">
         <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92">
-        <v>0</v>
-      </c>
-      <c r="B92" t="s">
-        <v>102</v>
-      </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
-      <c r="D92" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93">
-        <v>0</v>
-      </c>
-      <c r="B93" t="s">
-        <v>102</v>
-      </c>
-      <c r="C93">
-        <v>1</v>
-      </c>
-      <c r="D93" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94">
-        <v>0</v>
-      </c>
-      <c r="B94" t="s">
-        <v>102</v>
-      </c>
-      <c r="C94">
-        <v>1</v>
-      </c>
-      <c r="D94" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95">
-        <v>0</v>
-      </c>
-      <c r="B95" t="s">
-        <v>102</v>
-      </c>
-      <c r="C95">
-        <v>1</v>
-      </c>
-      <c r="D95" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96">
-        <v>0</v>
-      </c>
-      <c r="B96" t="s">
-        <v>102</v>
-      </c>
-      <c r="C96">
-        <v>1</v>
-      </c>
-      <c r="D96" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97">
-        <v>0</v>
-      </c>
-      <c r="B97" t="s">
-        <v>102</v>
-      </c>
-      <c r="C97">
-        <v>1</v>
-      </c>
-      <c r="D97" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98">
-        <v>0</v>
-      </c>
-      <c r="B98" t="s">
-        <v>102</v>
-      </c>
-      <c r="C98">
-        <v>1</v>
-      </c>
-      <c r="D98" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99">
-        <v>0</v>
-      </c>
-      <c r="B99" t="s">
-        <v>102</v>
-      </c>
-      <c r="C99">
-        <v>1</v>
-      </c>
-      <c r="D99" t="s">
-        <v>101</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D99" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D99">
-      <sortCondition ref="D1:D99"/>
-    </sortState>
-  </autoFilter>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>